<commit_message>
dangtq sửa thiết kế DB
</commit_message>
<xml_diff>
--- a/WIP/Analysis/CÁC VẤN ĐỀ CÒN TỒN ĐỘNG CỦA ATT ONLINE.xlsx
+++ b/WIP/Analysis/CÁC VẤN ĐỀ CÒN TỒN ĐỘNG CỦA ATT ONLINE.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Các Vấn Đề Còn Tồn Đọng  Trên Phần Mềm ATT Online Và Trách Nhiệm Của Các Bên</t>
   </si>
@@ -122,14 +117,37 @@
   </si>
   <si>
     <t>Yêu Cầu ATT xác nhận chấp nhận rủi ro khi mở tờ khai theo BCT scan</t>
+  </si>
+  <si>
+    <t>Phản hồi từ bộ phận Sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin PKD có trao đổi với chị Thảo kế toán để phản hồi về việc gửi link sau khi đã nộp thuế. </t>
+  </si>
+  <si>
+    <t>Sau khi đã nộp thuế và phí hãng tàu, thông tin sẽ được hiển thị ở phần dashboard (đã update)</t>
+  </si>
+  <si>
+    <t>Phần mềm đã update chức năng này</t>
+  </si>
+  <si>
+    <t>Khi sale chốt hàng, admin phòng bán đã cập nhật lên hệ thống để trừ tồn. Trừ trường hợp PKD chưa bán được thì chưa có kế hoạch. PKD đảm bảo không phát sinh hạn lưu cont lưu bãi khi đến hạn lưu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -172,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -193,13 +211,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -260,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -295,7 +323,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -472,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,31 +520,35 @@
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="90" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -529,8 +561,11 @@
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -543,8 +578,9 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -557,22 +593,28 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -585,8 +627,11 @@
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E8" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -599,8 +644,9 @@
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -611,8 +657,9 @@
         <v>31</v>
       </c>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="284.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -623,8 +670,9 @@
       <c r="D11" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -637,8 +685,9 @@
       <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -649,8 +698,9 @@
         <v>25</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -661,8 +711,9 @@
         <v>25</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -673,11 +724,13 @@
         <v>25</v>
       </c>
       <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>